<commit_message>
Issue #20: Printing the output of grep
</commit_message>
<xml_diff>
--- a/resources/heuristics-database.xlsx
+++ b/resources/heuristics-database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/db-mining/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D450D1-1971-5A42-A98E-B18A1D7A5553}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91DAF8E-F867-9F4B-AD9B-402D4F8A389F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{FF526B98-C890-C146-B149-2187E530C118}"/>
+    <workbookView xWindow="5440" yWindow="6180" windowWidth="27640" windowHeight="16940" xr2:uid="{FF526B98-C890-C146-B149-2187E530C118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>language</t>
   </si>
@@ -48,9 +48,6 @@
     <t>MySQL</t>
   </si>
   <si>
-    <t>jdbc:mysql:</t>
-  </si>
-  <si>
     <t>mysqlx:</t>
   </si>
   <si>
@@ -58,6 +55,48 @@
   </si>
   <si>
     <t>MySql.Data.MySqlClient.MySqlConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java </t>
+  </si>
+  <si>
+    <t>jdbc:hsqldb</t>
+  </si>
+  <si>
+    <t>jdbc:mysql</t>
+  </si>
+  <si>
+    <t>Derby</t>
+  </si>
+  <si>
+    <t>jdbc:derby</t>
+  </si>
+  <si>
+    <t>jdbc:h2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>jdbc:oracle</t>
+  </si>
+  <si>
+    <t>HyperSQL</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>case-sensitive</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>jdbc:postgresql</t>
   </si>
 </sst>
 </file>
@@ -116,9 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,19 +473,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B72D2D-FEFC-0949-A086-3162836F94F7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,10 +496,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -464,10 +513,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -475,18 +530,115 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>